<commit_message>
new functions and params of font and text location
</commit_message>
<xml_diff>
--- a/tests/data/data.xlsx
+++ b/tests/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ildar/Projects/git/text-to-image/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91136A5E-B46D-044C-9CBE-62809E595FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C640FF2-B5AA-0743-8859-34F4625DBAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{DD936D61-B7EE-D146-A653-FBAF8EE53B04}"/>
   </bookViews>
@@ -27,20 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Артикул</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Текст</t>
   </si>
   <si>
-    <t>Размер текста</t>
-  </si>
-  <si>
-    <t>Цвет</t>
-  </si>
-  <si>
     <t>Хвала безумцам, одиночкам, бунтарям, белым воронам, тем кто всегда некстати и невпопад, тем кто видит мир иначе. Они не соблюдают правил, они смеются над устоями, их можно цитировать, спорить с ними, восхвалять или проклинать их, но только игнорировать их - невозможно.</t>
   </si>
   <si>
@@ -60,6 +51,57 @@
   </si>
   <si>
     <t>черный</t>
+  </si>
+  <si>
+    <t>Файл с расшеринием</t>
+  </si>
+  <si>
+    <t>Колво символов (ДЛСТР)</t>
+  </si>
+  <si>
+    <t>Верх/Низ</t>
+  </si>
+  <si>
+    <t>Центровка текста по горизонтали</t>
+  </si>
+  <si>
+    <t>Сдвиг по вертикали в пикселях</t>
+  </si>
+  <si>
+    <t>Цвет текста</t>
+  </si>
+  <si>
+    <t>Шрифт</t>
+  </si>
+  <si>
+    <t>Размер шрифта</t>
+  </si>
+  <si>
+    <t>Жирность</t>
+  </si>
+  <si>
+    <t>Доп блоком или нет</t>
+  </si>
+  <si>
+    <t>Цвет фона</t>
+  </si>
+  <si>
+    <t>1.jpg</t>
+  </si>
+  <si>
+    <t>Arial</t>
+  </si>
+  <si>
+    <t>белый</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>3.jpg</t>
+  </si>
+  <si>
+    <t>4.jpg</t>
   </si>
 </sst>
 </file>
@@ -74,20 +116,30 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF96D0FF"/>
-      <name val="Fira Code"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,13 +147,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,82 +504,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F47F90-645D-9C4A-83DE-B3105CF07F82}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:12" ht="64">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7">
+        <v>30</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7">
+        <v>40</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>30</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7">
+        <v>50</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+    <row r="5" spans="1:12">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F5" s="7">
+        <v>100</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7">
+        <v>60</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="C5">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>